<commit_message>
A lot of work done on the Importing of data
</commit_message>
<xml_diff>
--- a/Excel/TestSheet.xlsx
+++ b/Excel/TestSheet.xlsx
@@ -8,14 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\AutoSheet\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB89AB4-F0CE-4ED7-BF3D-6F48DF26E972}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2912A20-CB53-423D-AF6A-AE5BF4764D36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25725" yWindow="1185" windowWidth="21600" windowHeight="14445" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13470" yWindow="2535" windowWidth="21600" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PipeDataXlOut" sheetId="1" r:id="rId1"/>
     <sheet name="PipeDataXlIn" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="PipeDataXlIn">PipeDataXlIn!$1:$1000</definedName>
+    <definedName name="PipeDataXlIn.EndInvert">PipeDataXlIn!$H:$H</definedName>
+    <definedName name="PipeDataXlIn.From">PipeDataXlIn!$B:$B</definedName>
+    <definedName name="PipeDataXlIn.Handle">PipeDataXlIn!$A:$A</definedName>
+    <definedName name="PipeDataXlIn.InnerDiameter">PipeDataXlIn!$F:$F</definedName>
+    <definedName name="PipeDataXlIn.Length">PipeDataXlIn!$D:$D</definedName>
+    <definedName name="PipeDataXlIn.Slope">PipeDataXlIn!$E:$E</definedName>
+    <definedName name="PipeDataXlIn.StartInvert">PipeDataXlIn!$G:$G</definedName>
+    <definedName name="PipeDataXlIn.To">PipeDataXlIn!$C:$C</definedName>
+    <definedName name="PipeDataXlOut">PipeDataXlOut!$1:$1048576</definedName>
+    <definedName name="PipeDataXlOut.EndInvert">PipeDataXlOut!$M:$M</definedName>
+    <definedName name="PipeDataXlOut.Handle">PipeDataXlOut!$A:$A</definedName>
+    <definedName name="PipeDataXlOut.Slope">PipeDataXlOut!$E:$E</definedName>
+    <definedName name="PipeDataXlOut.StartInvert">PipeDataXlOut!$I:$I</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>From</t>
   </si>
@@ -49,39 +65,49 @@
     <t>InnerDiameter</t>
   </si>
   <si>
-    <t>UObvert</t>
-  </si>
-  <si>
-    <t>UInvert</t>
-  </si>
-  <si>
-    <t>UCenterline</t>
-  </si>
-  <si>
-    <t>DCenterline</t>
-  </si>
-  <si>
-    <t>DObverDrop</t>
-  </si>
-  <si>
-    <t>DObvert</t>
-  </si>
-  <si>
-    <t>DInvert</t>
-  </si>
-  <si>
     <t>Handle</t>
   </si>
   <si>
-    <t>length</t>
+    <t>StartInvert</t>
+  </si>
+  <si>
+    <t>EndInvert</t>
+  </si>
+  <si>
+    <t>StartCenterline</t>
+  </si>
+  <si>
+    <t>StartObvert</t>
+  </si>
+  <si>
+    <t>EndCenterline</t>
+  </si>
+  <si>
+    <t>EndObvertDrop</t>
+  </si>
+  <si>
+    <t>EndObvert</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -128,7 +154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -137,6 +163,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -420,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,7 +474,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -451,97 +492,456 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="1">
-        <v>100</v>
-      </c>
-      <c r="C2" s="1">
-        <v>101</v>
+      <c r="A2" s="1">
+        <f>PipeDataXlIn!A2</f>
+        <v>27403</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f t="shared" ref="B2:B4" si="0">VLOOKUP($A2,PipeDataXlIn,COLUMN(PipeDataXlIn.From),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f t="shared" ref="C2:C4" si="1">VLOOKUP($A2,PipeDataXlIn,COLUMN(PipeDataXlIn.To),FALSE)</f>
+        <v>2</v>
       </c>
       <c r="D2" s="1">
-        <v>100</v>
+        <f t="shared" ref="D2:D4" si="2">VLOOKUP($A2,PipeDataXlIn,COLUMN(PipeDataXlIn.Length),FALSE)</f>
+        <v>184.43851621473189</v>
       </c>
       <c r="E2" s="2">
         <v>3.5000000000000001E-3</v>
       </c>
       <c r="F2" s="1">
-        <v>1200</v>
-      </c>
-      <c r="H2" s="1">
+        <v>200</v>
+      </c>
+      <c r="H2" s="8">
         <f>I2+F2/1000</f>
-        <v>109.89999999999999</v>
-      </c>
-      <c r="I2" s="1">
+        <v>112.61924780290242</v>
+      </c>
+      <c r="I2" s="8">
         <f>M2+E2*D2</f>
-        <v>108.69999999999999</v>
-      </c>
-      <c r="L2" s="1">
+        <v>112.41924780290242</v>
+      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8">
+        <v>0.59</v>
+      </c>
+      <c r="L2" s="8">
         <f>H3+K2</f>
-        <v>109.55</v>
-      </c>
-      <c r="M2" s="1">
+        <v>111.97371299615087</v>
+      </c>
+      <c r="M2" s="8">
         <f>L2-F2/1000</f>
-        <v>108.35</v>
+        <v>111.77371299615086</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
-        <v>101</v>
-      </c>
-      <c r="C3" s="1">
-        <v>102</v>
+      <c r="A3" s="1">
+        <f>PipeDataXlIn!A3</f>
+        <v>27427</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="D3" s="1">
-        <v>100</v>
+        <f t="shared" si="2"/>
+        <v>75.942801559227519</v>
       </c>
       <c r="E3" s="2">
         <v>3.5000000000000001E-3</v>
       </c>
       <c r="F3" s="1">
-        <v>1200</v>
-      </c>
-      <c r="H3" s="1">
+        <v>200</v>
+      </c>
+      <c r="H3" s="8">
         <f>I3+F3/1000</f>
-        <v>109.55</v>
-      </c>
-      <c r="I3" s="1">
+        <v>111.38371299615086</v>
+      </c>
+      <c r="I3" s="8">
         <f>M3+E3*D3</f>
-        <v>108.35</v>
-      </c>
-      <c r="L3" s="1">
+        <v>111.18371299615086</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8">
+        <v>0.59</v>
+      </c>
+      <c r="L3" s="8">
         <f>H4+K3</f>
-        <v>120</v>
-      </c>
-      <c r="M3" s="1">
-        <f>L3-F3/100</f>
-        <v>108</v>
+        <v>111.11791319069357</v>
+      </c>
+      <c r="M3" s="8">
+        <f>L3-F3/1000</f>
+        <v>110.91791319069357</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H4" s="1">
-        <v>120</v>
-      </c>
+      <c r="A4" s="1">
+        <f>PipeDataXlIn!A4</f>
+        <v>27442</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="2"/>
+        <v>150.83234019816155</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>200</v>
+      </c>
+      <c r="H4" s="8">
+        <f>I4+F4/1000</f>
+        <v>110.52791319069357</v>
+      </c>
+      <c r="I4" s="8">
+        <f>M4+E4*D4</f>
+        <v>110.32791319069356</v>
+      </c>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8">
+        <f>110+K4</f>
+        <v>110</v>
+      </c>
+      <c r="M4" s="8">
+        <f>L4-F4/1000</f>
+        <v>109.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E5" s="2"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E6" s="2"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E7" s="2"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E8" s="2"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E9" s="2"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E10" s="2"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E11" s="2"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E12" s="2"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E13" s="2"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E14" s="2"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E15" s="2"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+    </row>
+    <row r="21" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+    </row>
+    <row r="23" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+    </row>
+    <row r="24" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+    </row>
+    <row r="25" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+    </row>
+    <row r="26" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+    </row>
+    <row r="27" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+    </row>
+    <row r="28" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+    </row>
+    <row r="29" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+    </row>
+    <row r="30" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+    </row>
+    <row r="31" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+    </row>
+    <row r="32" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+    </row>
+    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+    </row>
+    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+    </row>
+    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+    </row>
+    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+    </row>
+    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+    </row>
+    <row r="38" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+    </row>
+    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+    </row>
+    <row r="40" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -551,105 +951,161 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1352CDF2-BF75-4251-A393-CC8669F8CA5D}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="16.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.140625" style="7"/>
+    <col min="6" max="6" width="16.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>27403</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>27120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1">
+        <v>184.43851621473189</v>
+      </c>
+      <c r="E2" s="7">
+        <v>3.4999999999999688E-3</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>112.41924780290242</v>
+      </c>
+      <c r="H2" s="1">
+        <v>111.77371299615086</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>27144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27427</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1">
+        <v>75.942801559227519</v>
+      </c>
+      <c r="E3" s="7">
+        <v>3.4999999999999355E-3</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>111.18371299615086</v>
+      </c>
+      <c r="H3" s="1">
+        <v>110.91791319069357</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>27159</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>27183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>27261</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>27285</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>27309</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>27333</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>27357</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>27381</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>27405</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>27429</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>27453</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>27477</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>27501</v>
-      </c>
+        <v>27442</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1">
+        <v>150.83234019816155</v>
+      </c>
+      <c r="E4" s="7">
+        <v>3.5000000000000135E-3</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>110.32791319069356</v>
+      </c>
+      <c r="H4" s="1">
+        <v>109.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Trying out the release build and updating the startup script
</commit_message>
<xml_diff>
--- a/Excel/TestSheet.xlsx
+++ b/Excel/TestSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\AutoSheet\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2912A20-CB53-423D-AF6A-AE5BF4764D36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5062A75D-6E2D-43BC-BFC5-9D2AD63E283C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13470" yWindow="2535" windowWidth="21600" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22050" yWindow="2865" windowWidth="21600" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PipeDataXlOut" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,18 +531,18 @@
         <v>184.43851621473189</v>
       </c>
       <c r="E2" s="2">
-        <v>3.5000000000000001E-3</v>
+        <v>0.02</v>
       </c>
       <c r="F2" s="1">
         <v>200</v>
       </c>
       <c r="H2" s="8">
         <f>I2+F2/1000</f>
-        <v>112.61924780290242</v>
+        <v>116.39691664343739</v>
       </c>
       <c r="I2" s="8">
         <f>M2+E2*D2</f>
-        <v>112.41924780290242</v>
+        <v>116.19691664343739</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8">
@@ -550,11 +550,11 @@
       </c>
       <c r="L2" s="8">
         <f>H3+K2</f>
-        <v>111.97371299615087</v>
+        <v>112.70814631914276</v>
       </c>
       <c r="M2" s="8">
         <f>L2-F2/1000</f>
-        <v>111.77371299615086</v>
+        <v>112.50814631914275</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -575,18 +575,18 @@
         <v>75.942801559227519</v>
       </c>
       <c r="E3" s="2">
-        <v>3.5000000000000001E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="F3" s="1">
         <v>200</v>
       </c>
       <c r="H3" s="8">
         <f>I3+F3/1000</f>
-        <v>111.38371299615086</v>
+        <v>112.11814631914275</v>
       </c>
       <c r="I3" s="8">
         <f>M3+E3*D3</f>
-        <v>111.18371299615086</v>
+        <v>111.91814631914275</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8">
@@ -594,11 +594,11 @@
       </c>
       <c r="L3" s="8">
         <f>H4+K3</f>
-        <v>111.11791319069357</v>
+        <v>111.43466110510971</v>
       </c>
       <c r="M3" s="8">
         <f>L3-F3/1000</f>
-        <v>110.91791319069357</v>
+        <v>111.23466110510971</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -619,18 +619,18 @@
         <v>150.83234019816155</v>
       </c>
       <c r="E4" s="2">
-        <v>3.5000000000000001E-3</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="F4" s="1">
         <v>200</v>
       </c>
       <c r="H4" s="8">
         <f>I4+F4/1000</f>
-        <v>110.52791319069357</v>
+        <v>110.84466110510971</v>
       </c>
       <c r="I4" s="8">
         <f>M4+E4*D4</f>
-        <v>110.32791319069356</v>
+        <v>110.64466110510971</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
@@ -1016,10 +1016,10 @@
         <v>0.2</v>
       </c>
       <c r="G2" s="1">
-        <v>112.41924780290242</v>
+        <v>112.5416499038825</v>
       </c>
       <c r="H2" s="1">
-        <v>111.77371299615086</v>
+        <v>111.89611509713095</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1042,10 +1042,10 @@
         <v>0.2</v>
       </c>
       <c r="G3" s="1">
-        <v>111.18371299615086</v>
+        <v>111.30611509713094</v>
       </c>
       <c r="H3" s="1">
-        <v>110.91791319069357</v>
+        <v>111.04031529167365</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1062,13 +1062,13 @@
         <v>150.83234019816155</v>
       </c>
       <c r="E4" s="7">
-        <v>3.5000000000000135E-3</v>
+        <v>4.3115109851062042E-3</v>
       </c>
       <c r="F4" s="8">
         <v>0.2</v>
       </c>
       <c r="G4" s="1">
-        <v>110.32791319069356</v>
+        <v>110.45031529167365</v>
       </c>
       <c r="H4" s="1">
         <v>109.8</v>

</xml_diff>

<commit_message>
Cleaning a lot of things up and fixing issue where excel would keep running in the back ground
</commit_message>
<xml_diff>
--- a/Excel/TestSheet.xlsx
+++ b/Excel/TestSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\AutoSheet\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5062A75D-6E2D-43BC-BFC5-9D2AD63E283C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD227381-F6AF-4BB8-BA02-DBA8B186574F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22050" yWindow="2865" windowWidth="21600" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20940" yWindow="2700" windowWidth="21600" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PipeDataXlOut" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,16 +1010,16 @@
         <v>184.43851621473189</v>
       </c>
       <c r="E2" s="7">
-        <v>3.4999999999999688E-3</v>
+        <v>1.9999999999999997E-2</v>
       </c>
       <c r="F2" s="8">
         <v>0.2</v>
       </c>
       <c r="G2" s="1">
-        <v>112.5416499038825</v>
+        <v>116.19691664343739</v>
       </c>
       <c r="H2" s="1">
-        <v>111.89611509713095</v>
+        <v>112.50814631914275</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1036,16 +1036,16 @@
         <v>75.942801559227519</v>
       </c>
       <c r="E3" s="7">
-        <v>3.4999999999999355E-3</v>
+        <v>8.9999999999999143E-3</v>
       </c>
       <c r="F3" s="8">
         <v>0.2</v>
       </c>
       <c r="G3" s="1">
-        <v>111.30611509713094</v>
+        <v>111.91814631914275</v>
       </c>
       <c r="H3" s="1">
-        <v>111.04031529167365</v>
+        <v>111.23466110510971</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1062,13 +1062,13 @@
         <v>150.83234019816155</v>
       </c>
       <c r="E4" s="7">
-        <v>4.3115109851062042E-3</v>
+        <v>5.6000000000000216E-3</v>
       </c>
       <c r="F4" s="8">
         <v>0.2</v>
       </c>
       <c r="G4" s="1">
-        <v>110.45031529167365</v>
+        <v>110.64466110510971</v>
       </c>
       <c r="H4" s="1">
         <v>109.8</v>

</xml_diff>